<commit_message>
Started on interrupt handler
</commit_message>
<xml_diff>
--- a/Configuration.xlsx
+++ b/Configuration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvone\Desktop\Engineering 3\Design (E) - 314\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21785155\Documents\edesign_2020_21785155\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB771446-5A94-49C4-915B-2CB47F85608F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3140147-353C-4664-93BC-D537699FF71C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1CFFCA70-AF03-40EA-B3C0-8716D8FC6C47}"/>
   </bookViews>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Stop</t>
   </si>
@@ -82,6 +76,21 @@
   </si>
   <si>
     <t>J3 - 9,10</t>
+  </si>
+  <si>
+    <t>EXTI8</t>
+  </si>
+  <si>
+    <t>EXTI6</t>
+  </si>
+  <si>
+    <t>EXTI7</t>
+  </si>
+  <si>
+    <t>EXTI10</t>
+  </si>
+  <si>
+    <t>EXTI9</t>
   </si>
 </sst>
 </file>
@@ -132,10 +141,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,167 +470,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9FE4D2-09B3-484D-8212-A0A31BF2A377}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="E3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="E4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Started on enums and interrupts
</commit_message>
<xml_diff>
--- a/Configuration.xlsx
+++ b/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21785155\Documents\edesign_2020_21785155\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3140147-353C-4664-93BC-D537699FF71C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A0C93D-4D89-4021-BE3B-8763B39F1F37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1CFFCA70-AF03-40EA-B3C0-8716D8FC6C47}"/>
   </bookViews>
@@ -473,10 +473,13 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">

</xml_diff>